<commit_message>
First commit, migrating project to GitHub
</commit_message>
<xml_diff>
--- a/docs/Structure.xlsx
+++ b/docs/Structure.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sokram\Documents\Proyectos\gauge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA366247-2BD0-44ED-B852-4FEF7E01157B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E7CAD2-5054-40CC-BF20-73DB72AC980D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{D17A02BD-AB55-449C-AFDA-916FFCBC1C76}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{D17A02BD-AB55-449C-AFDA-916FFCBC1C76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="5">
   <si>
     <t>MEDIDOR</t>
   </si>
@@ -252,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -272,12 +273,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -293,36 +288,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -335,10 +300,64 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -660,154 +679,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0187A774-D4A7-40ED-B361-3FB881345DE3}">
-  <dimension ref="B1:J10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="D1" s="2">
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="E1" s="2">
+      <c r="D1" s="4">
         <v>2</v>
       </c>
-      <c r="F1" s="2">
+      <c r="E1" s="4">
         <v>3</v>
       </c>
-      <c r="G1" s="2">
+      <c r="F1" s="4">
         <v>4</v>
       </c>
-      <c r="H1" s="2">
+      <c r="G1" s="4">
         <v>5</v>
       </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
       <c r="I1" s="2">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="34">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="9" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="5"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="34"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
         <v>1</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="5"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="16"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="34"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="5"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -831,23 +852,179 @@
       <c r="I10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:E9"/>
-    <mergeCell ref="F6:G9"/>
-    <mergeCell ref="H6:I9"/>
-    <mergeCell ref="E2:F5"/>
-    <mergeCell ref="G2:H5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C6:D9"/>
+    <mergeCell ref="D2:E5"/>
+    <mergeCell ref="F2:G5"/>
+    <mergeCell ref="E6:F9"/>
+    <mergeCell ref="G6:H9"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E3573-5D85-4814-AE00-C01A99E00950}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D2:E5"/>
+    <mergeCell ref="F2:G5"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="C6:D9"/>
+    <mergeCell ref="E6:F9"/>
+    <mergeCell ref="G6:H9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>